<commit_message>
All Winters animations pass validation of new schema
</commit_message>
<xml_diff>
--- a/animations/2019 IWP Animations.xlsx
+++ b/animations/2019 IWP Animations.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/brockman/ncssm/git/iwphys/animations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{6993D379-8579-754B-A06D-2A0D278125D4}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{9FDF602B-458A-F347-BDDD-72C15EE9D06F}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4460" yWindow="-19420" windowWidth="28040" windowHeight="17040"/>
+    <workbookView xWindow="340" yWindow="460" windowWidth="28040" windowHeight="17040"/>
   </bookViews>
   <sheets>
     <sheet name="2019 IWP Animations" sheetId="1" r:id="rId1"/>
@@ -3187,9 +3187,6 @@
     <t>http://localhost:8470/valiation/unit-test-2017/TEST_euler.iwp</t>
   </si>
   <si>
-    <t>Double Rounding</t>
-  </si>
-  <si>
     <t>IWP Json Animation</t>
   </si>
   <si>
@@ -3197,6 +3194,9 @@
   </si>
   <si>
     <t>Testing Results</t>
+  </si>
+  <si>
+    <t>Double Rounding Precision</t>
   </si>
 </sst>
 </file>
@@ -4064,25 +4064,25 @@
   <dimension ref="A1:C1055"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="65.33203125" customWidth="1"/>
     <col min="2" max="2" width="55.83203125" customWidth="1"/>
-    <col min="3" max="3" width="17.83203125" customWidth="1"/>
+    <col min="3" max="3" width="26.33203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
+        <v>1055</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>1056</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>1057</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>1058</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -4103,7 +4103,7 @@
         <v>1054</v>
       </c>
       <c r="C4" t="s">
-        <v>1055</v>
+        <v>1058</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>